<commit_message>
edits to shared reward behavioral analysis code
</commit_message>
<xml_diff>
--- a/Shared_Reward/Behavioral_Analysis/age & gender.xlsx
+++ b/Shared_Reward/Behavioral_Analysis/age & gender.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>sub</t>
   </si>
@@ -34,12 +34,15 @@
   <si>
     <t>gender</t>
   </si>
+  <si>
+    <t>1001, 1006, 1009, 1010, 1011, 1012, 1013, 1015, 1016, 1019, 1021, 1242, 1243, 1244, 1248, 1249, 1251, 1255, 1276, 1282, 1286, 1294, 1301, 1302, 1303, 3116, 3122, 3125, 3140, 3143, 3152, 3166, 3167, 3170, 3173, 3176, 3189, 3190, 3199, 3200, 3206, 3210, 3212, 3218, 3220</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +56,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,15 +88,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -358,13 +378,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,7 +397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -385,679 +407,647 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>1001</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="B3" s="1">
-        <v>21.205479449999999</v>
+        <v>20.72054795</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>1003</v>
+        <v>1009</v>
       </c>
       <c r="B4" s="1">
-        <v>19.05753425</v>
+        <v>20.203015799999999</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="B5" s="1">
-        <v>19.07123288</v>
+        <v>22.215377449999998</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="B6" s="1">
-        <v>20.72054795</v>
+        <v>21.979917449999999</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>1007</v>
+        <v>1012</v>
       </c>
       <c r="B7" s="1">
-        <v>21.23520675</v>
+        <v>22.064792570000002</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="B8" s="1">
-        <v>20.203015799999999</v>
+        <v>18.579551030000001</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>1010</v>
+        <v>1015</v>
       </c>
       <c r="B9" s="1">
-        <v>22.215377449999998</v>
+        <v>21.552918040000002</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>1011</v>
+        <v>1016</v>
       </c>
       <c r="B10" s="1">
-        <v>21.979917449999999</v>
+        <v>22.13871606</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>1012</v>
+        <v>1019</v>
       </c>
       <c r="B11" s="1">
-        <v>22.064792570000002</v>
+        <v>18.234460670000001</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>1013</v>
+        <v>1021</v>
       </c>
       <c r="B12" s="1">
-        <v>18.579551030000001</v>
+        <v>21.19687605</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>1015</v>
+        <v>1242</v>
       </c>
       <c r="B13" s="1">
-        <v>21.552918040000002</v>
+        <v>20.033265570000001</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>1016</v>
+        <v>1243</v>
       </c>
       <c r="B14" s="1">
-        <v>22.13871606</v>
+        <v>24.641048980000001</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>1018</v>
+        <v>1244</v>
       </c>
       <c r="B15" s="1">
-        <v>20.54263035</v>
+        <v>26.28105528</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>1019</v>
+        <v>1248</v>
       </c>
       <c r="B16" s="1">
-        <v>18.234460670000001</v>
+        <v>23.523982920000002</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>1021</v>
+        <v>1249</v>
       </c>
       <c r="B17" s="1">
-        <v>21.19687605</v>
+        <v>19.359626370000001</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>1240</v>
+        <v>1251</v>
       </c>
       <c r="B18" s="1">
-        <v>21.415794529999999</v>
+        <v>21.884090709999999</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>1242</v>
+        <v>1255</v>
       </c>
       <c r="B19" s="1">
-        <v>20.033265570000001</v>
+        <v>19.87172906</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>1243</v>
+        <v>1276</v>
       </c>
       <c r="B20" s="1">
-        <v>24.641048980000001</v>
+        <v>21.00522256</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>1244</v>
+        <v>1282</v>
       </c>
       <c r="B21" s="1">
-        <v>26.28105528</v>
+        <v>20.326107539999999</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>1245</v>
+        <v>1286</v>
       </c>
       <c r="B22" s="1">
-        <v>20.835472320000001</v>
+        <v>22.683445469999999</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>1247</v>
+        <v>1294</v>
       </c>
       <c r="B23" s="1">
-        <v>20.986057209999998</v>
+        <v>21.71160257</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>1248</v>
+        <v>1301</v>
       </c>
       <c r="B24" s="1">
-        <v>23.523982920000002</v>
+        <v>23.44458362</v>
       </c>
       <c r="C24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>1249</v>
+        <v>1302</v>
       </c>
       <c r="B25" s="1">
-        <v>19.359626370000001</v>
+        <v>23.020322109999999</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>1251</v>
+        <v>1303</v>
       </c>
       <c r="B26" s="1">
-        <v>21.884090709999999</v>
+        <v>19.934586840000001</v>
       </c>
       <c r="C26" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>1253</v>
+        <v>3116</v>
       </c>
       <c r="B27" s="1">
-        <v>19.176300680000001</v>
+        <v>20.123616500000001</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>1255</v>
+        <v>3122</v>
       </c>
       <c r="B28" s="1">
-        <v>19.87172906</v>
+        <v>20.840948139999998</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <v>3122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>1276</v>
+        <v>3125</v>
       </c>
       <c r="B29" s="1">
-        <v>21.00522256</v>
+        <v>21.766360710000001</v>
       </c>
       <c r="C29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>1282</v>
+        <v>3140</v>
       </c>
       <c r="B30" s="1">
-        <v>20.326107539999999</v>
+        <v>23.07781816</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <v>3140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>1286</v>
+        <v>3143</v>
       </c>
       <c r="B31" s="1">
-        <v>22.683445469999999</v>
+        <v>20.95867814</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <v>3143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>1294</v>
+        <v>3152</v>
       </c>
       <c r="B32" s="1">
-        <v>21.71160257</v>
+        <v>22.573929190000001</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>1300</v>
+        <v>3166</v>
       </c>
       <c r="B33" s="1">
-        <v>20.38634149</v>
+        <v>21.478766390000001</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <v>3166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>1301</v>
+        <v>3167</v>
       </c>
       <c r="B34" s="1">
-        <v>23.44458362</v>
+        <v>21.837432209999999</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>1302</v>
+        <v>3170</v>
       </c>
       <c r="B35" s="1">
-        <v>23.020322109999999</v>
+        <v>19.781264050000001</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>1303</v>
+        <v>3173</v>
       </c>
       <c r="B36" s="1">
-        <v>19.934586840000001</v>
+        <v>18.483496120000002</v>
       </c>
       <c r="C36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>3101</v>
+        <v>3176</v>
       </c>
       <c r="B37" s="1">
-        <v>22.259183969999999</v>
+        <v>19.321409750000001</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <v>3176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>3116</v>
+        <v>3189</v>
       </c>
       <c r="B38" s="1">
-        <v>20.123616500000001</v>
+        <v>23.439221889999999</v>
       </c>
       <c r="C38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2">
+        <v>3189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>3122</v>
+        <v>3190</v>
       </c>
       <c r="B39" s="1">
-        <v>20.840948139999998</v>
+        <v>19.718292179999999</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <v>3190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>3125</v>
+        <v>3199</v>
       </c>
       <c r="B40" s="1">
-        <v>21.766360710000001</v>
+        <v>20.071596270000001</v>
       </c>
       <c r="C40" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>3140</v>
+        <v>3200</v>
       </c>
       <c r="B41" s="1">
-        <v>23.07781816</v>
+        <v>18.215295319999999</v>
       </c>
       <c r="C41" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>3143</v>
+        <v>3206</v>
       </c>
       <c r="B42" s="1">
-        <v>20.95867814</v>
+        <v>19.252962069999999</v>
       </c>
       <c r="C42" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D42" s="2">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>3146</v>
+        <v>3210</v>
       </c>
       <c r="B43" s="1">
-        <v>19.58413474</v>
+        <v>18.18517834</v>
       </c>
       <c r="C43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>3152</v>
+        <v>3212</v>
       </c>
       <c r="B44" s="1">
-        <v>22.573929190000001</v>
+        <v>19.12154254</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <v>3212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>3164</v>
+        <v>3218</v>
       </c>
       <c r="B45" s="1">
-        <v>20.755958939999999</v>
+        <v>23.428384340000001</v>
       </c>
       <c r="C45" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <v>3218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>3166</v>
+        <v>3220</v>
       </c>
       <c r="B46" s="1">
-        <v>21.478766390000001</v>
+        <v>22.426310369999999</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>3167</v>
-      </c>
-      <c r="B47" s="1">
-        <v>21.837432209999999</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>3170</v>
-      </c>
-      <c r="B48" s="1">
-        <v>19.781264050000001</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>3173</v>
-      </c>
-      <c r="B49" s="1">
-        <v>18.483496120000002</v>
-      </c>
-      <c r="C49" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>3175</v>
-      </c>
-      <c r="B50" s="1">
-        <v>18.42337625</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>3176</v>
-      </c>
-      <c r="B51" s="1">
-        <v>19.321409750000001</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>3178</v>
-      </c>
-      <c r="B52" s="1">
-        <v>20.605374059999999</v>
-      </c>
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>3186</v>
-      </c>
-      <c r="B53" s="1">
-        <v>18.5519438</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>3189</v>
-      </c>
-      <c r="B54" s="1">
-        <v>23.439221889999999</v>
-      </c>
-      <c r="C54" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>3190</v>
-      </c>
-      <c r="B55" s="1">
-        <v>19.718292179999999</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>3199</v>
-      </c>
-      <c r="B56" s="1">
-        <v>20.071596270000001</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>3200</v>
-      </c>
-      <c r="B57" s="1">
-        <v>18.215295319999999</v>
-      </c>
-      <c r="C57" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>3206</v>
-      </c>
-      <c r="B58" s="1">
-        <v>19.252962069999999</v>
-      </c>
-      <c r="C58" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>3210</v>
-      </c>
-      <c r="B59" s="1">
-        <v>18.18517834</v>
-      </c>
-      <c r="C59" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>3212</v>
-      </c>
-      <c r="B60" s="1">
-        <v>19.12154254</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>3218</v>
-      </c>
-      <c r="B61" s="1">
-        <v>23.428384340000001</v>
-      </c>
-      <c r="C61" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="D46" s="2">
         <v>3220</v>
       </c>
-      <c r="B62" s="1">
-        <v>22.426310369999999</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>3223</v>
-      </c>
-      <c r="B63" s="1">
-        <v>19.55698383</v>
-      </c>
-      <c r="C63" s="1">
-        <v>1</v>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <f>AVERAGE(B2:B46)</f>
+        <v>21.112627765777777</v>
+      </c>
+      <c r="C47" s="3">
+        <f>COUNTIF(C2:C46, "2")/COUNTIF(C2:C46, "1")</f>
+        <v>0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <f>_xlfn.STDEV.S(B2:B46)</f>
+        <v>1.8348089269976962</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>